<commit_message>
Changed site_topic to source_topic; added region to cad legislator row
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\IOTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84D7857-6BB3-441C-BD94-73821DF83466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538C57D3-C2EE-4FB0-B6FF-238ECEF45C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="306">
   <si>
     <t>http://www.legislature.state.al.us/aliswww/ISD/ALRepresentative.aspx?NAME=Dismukes&amp;OID_SPONSOR=100570&amp;OID_PERSON=8511</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Role of the legislator</t>
   </si>
   <si>
-    <t>Senator, Representative</t>
-  </si>
-  <si>
     <t>The years the legislator has been active. If a range is given, all years in the range are to be listed.</t>
   </si>
   <si>
@@ -542,18 +539,6 @@
     <t>United States of America, Canada</t>
   </si>
   <si>
-    <t>Char(2)</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>US Postal Code abbreviation for a given state</t>
-  </si>
-  <si>
-    <t>TX, OH</t>
-  </si>
-  <si>
     <t>Examples</t>
   </si>
   <si>
@@ -623,9 +608,6 @@
     <t>date_introduced</t>
   </si>
   <si>
-    <t>site_topic</t>
-  </si>
-  <si>
     <t>topic</t>
   </si>
   <si>
@@ -680,38 +662,6 @@
     <t>bill_description</t>
   </si>
   <si>
-    <r>
-      <t>Generated by database. ID of the bill state of origin. Can be found by querying the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> us_state_info</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> table and joining the .</t>
-    </r>
-  </si>
-  <si>
-    <t>Two character US Postal code abbreviation depicting the name of the state.</t>
-  </si>
-  <si>
-    <t>IL</t>
-  </si>
-  <si>
     <t>Type of bill.</t>
   </si>
   <si>
@@ -809,9 +759,6 @@
   </si>
   <si>
     <t>District of the legislator, typically represented as a number. Be sure to remove and ordinal indicators and the word "District" if present. So if a legislator has their district as "District 42" or "42nd District", it should just be represented as "42".</t>
-  </si>
-  <si>
-    <t>Legislator party. Be sure to use full name of the party, if available.</t>
   </si>
   <si>
     <t>[{role: X, committee: X}, ...]</t>
@@ -873,32 +820,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Generated by database. FIPS code of a given state. Can be acquired by querying the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">us_state_info </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>table.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Generated by database. ID for a give party. Can be acquired by querying the </t>
     </r>
     <r>
@@ -933,13 +854,7 @@
     <t>goverlytics_id (PRIMARY KEY)</t>
   </si>
   <si>
-    <t>state_member_id</t>
-  </si>
-  <si>
     <t>most_recent_term_id</t>
-  </si>
-  <si>
-    <t>ID of legislator provided by the state website</t>
   </si>
   <si>
     <t>ID of the most recent term where the legislator was elected</t>
@@ -1097,6 +1012,33 @@
   </si>
   <si>
     <t>state_id changed to source_id</t>
+  </si>
+  <si>
+    <t>riding</t>
+  </si>
+  <si>
+    <t>Riding served by the legislator</t>
+  </si>
+  <si>
+    <t>Prince Albert, Toronto-St Paul's</t>
+  </si>
+  <si>
+    <t>ID of legislator provided by the source material</t>
+  </si>
+  <si>
+    <t>Legislator party. Use full name of party.</t>
+  </si>
+  <si>
+    <t>Senator, Representative, Member of Parliament</t>
+  </si>
+  <si>
+    <t>source_topic</t>
+  </si>
+  <si>
+    <t>site_topic change to source_topic</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -1375,6 +1317,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1408,39 +1356,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1617,6 +1532,39 @@
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1631,27 +1579,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E30" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:E30" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:E26" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2003,7 +1951,7 @@
         <v>61</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>5</v>
@@ -2050,7 +1998,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>9</v>
@@ -2068,7 +2016,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O2" s="16"/>
     </row>
@@ -2113,7 +2061,7 @@
         <v>34</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O3" s="16"/>
     </row>
@@ -2158,7 +2106,7 @@
         <v>34</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>35</v>
@@ -2205,7 +2153,7 @@
         <v>34</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O5" s="16" t="s">
         <v>33</v>
@@ -2255,7 +2203,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>9</v>
@@ -2273,7 +2221,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>41</v>
@@ -2345,7 +2293,7 @@
         <v>20</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>51</v>
@@ -2390,7 +2338,7 @@
         <v>34</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>55</v>
@@ -2398,13 +2346,13 @@
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
@@ -2435,21 +2383,21 @@
         <v>34</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
@@ -2462,7 +2410,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>9</v>
@@ -2480,24 +2428,24 @@
         <v>20</v>
       </c>
       <c r="N12" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>127</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>9</v>
@@ -2527,15 +2475,15 @@
         <v>34</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>37</v>
@@ -2556,16 +2504,16 @@
     </row>
     <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>131</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -2581,13 +2529,13 @@
     </row>
     <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
@@ -2618,21 +2566,21 @@
         <v>9</v>
       </c>
       <c r="N16" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>138</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>139</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
@@ -2663,21 +2611,21 @@
         <v>34</v>
       </c>
       <c r="N17" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>141</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>142</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16" t="s">
@@ -2690,7 +2638,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>9</v>
@@ -2708,21 +2656,21 @@
         <v>34</v>
       </c>
       <c r="N18" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
@@ -2735,39 +2683,39 @@
         <v>10</v>
       </c>
       <c r="H19" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="M19" s="16" t="s">
+      <c r="N19" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="O19" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
@@ -2780,7 +2728,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>9</v>
@@ -2798,21 +2746,21 @@
         <v>20</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>158</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>159</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16" t="s">
@@ -2840,13 +2788,13 @@
         <v>9</v>
       </c>
       <c r="M21" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="O21" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3132,10 +3080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3161,53 +3109,53 @@
         <v>69</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>105</v>
-      </c>
       <c r="D4" s="29" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E4" s="29">
         <v>43915</v>
@@ -3215,46 +3163,46 @@
     </row>
     <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>105</v>
-      </c>
       <c r="D7" s="29" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E7" s="29">
         <v>43853</v>
@@ -3262,32 +3210,32 @@
     </row>
     <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3295,447 +3243,413 @@
         <v>21</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>71</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="E11" s="29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>169</v>
-      </c>
+      <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>220</v>
+        <v>230</v>
+      </c>
+      <c r="E14" s="29">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>236</v>
+        <v>181</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="29"/>
+        <v>90</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>92</v>
+      </c>
       <c r="D16" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="E16" s="29">
-        <v>53</v>
+        <v>214</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>235</v>
+        <v>182</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="29"/>
+        <v>191</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>216</v>
+      </c>
       <c r="D17" s="29" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>93</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C20" s="29"/>
       <c r="D20" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>224</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>225</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C21" s="29"/>
       <c r="D21" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>226</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="29" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="29"/>
+        <v>91</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>223</v>
+      </c>
       <c r="D23" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="E23" s="29"/>
-    </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="24" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="29"/>
+        <v>91</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>262</v>
+      </c>
       <c r="D24" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="24" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>192</v>
+        <v>303</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="E25" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="E25" s="29" t="s">
+    </row>
+    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>240</v>
-      </c>
       <c r="E26" s="29" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>73</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>242</v>
+        <v>272</v>
+      </c>
+      <c r="E27" s="30">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E29" s="30">
+      <c r="B32" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="E32" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="B30" s="29" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="C33" s="33"/>
+      <c r="D33" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B36" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C36" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D36" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" s="32" t="s">
+      <c r="E36" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E37" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="E38" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="E34" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="E39" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="B40" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="E40" s="33" t="s">
-        <v>297</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E30">
+  <conditionalFormatting sqref="A1:E28">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33:E35">
+  <conditionalFormatting sqref="A31:E33">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A38:E40">
+  <conditionalFormatting sqref="A36:E38">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
@@ -3753,10 +3667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3783,12 +3697,12 @@
         <v>69</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>70</v>
@@ -3805,29 +3719,29 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>262</v>
+        <v>300</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="E4" s="4">
         <v>101</v>
@@ -3835,16 +3749,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E5" s="14">
         <v>43831</v>
@@ -3852,17 +3766,17 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3942,7 +3856,7 @@
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>10</v>
@@ -3951,7 +3865,7 @@
         <v>71</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -3959,22 +3873,22 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="7" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>282</v>
+        <v>163</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
@@ -3983,7 +3897,7 @@
         <v>71</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -3991,387 +3905,368 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>165</v>
+        <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>169</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>170</v>
+        <v>301</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>164</v>
+        <v>64</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>71</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="7"/>
+        <v>191</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="D17" s="7" t="s">
-        <v>250</v>
+        <v>86</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>241</v>
+      </c>
       <c r="D18" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>248</v>
+        <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="E19" s="7">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>197</v>
+        <v>91</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>251</v>
+        <v>73</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>252</v>
+        <v>97</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="10">
+        <v>24551</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="C25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>105</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="10">
-        <v>24551</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="D30" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="B30" s="7" t="s">
+    </row>
+    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
+      <c r="C33" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="34" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="E37" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" s="38" t="s">
+      <c r="E38" s="40" t="s">
         <v>284</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>298</v>
-      </c>
-      <c r="E34" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="E35" s="40" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>71</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C39" s="38"/>
       <c r="D39" s="38" t="s">
-        <v>300</v>
-      </c>
-      <c r="E39" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40" t="s">
-        <v>301</v>
-      </c>
-      <c r="E40" s="40" t="s">
-        <v>297</v>
+        <v>298</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A30:E30">
+  <conditionalFormatting sqref="A26:E26">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E25" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
-    <hyperlink ref="C25" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
+    <hyperlink ref="E21" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
+    <hyperlink ref="C21" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4383,10 +4278,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C073D259-A667-418B-8FFC-7962EC73964E}">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4396,147 +4291,155 @@
   <sheetData>
     <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q30" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>309</v>
+    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>307</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued work on CAD fed legislator scraper
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049E21E-2434-4623-BF7A-E86E22822A67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DFA2C1-0005-4B2F-AED3-71B866FF7FC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
@@ -1339,34 +1339,6 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1542,6 +1514,13 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1574,6 +1553,27 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1588,27 +1588,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E26" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3649,17 +3649,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E28">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:E33">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:E38">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3678,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,7 +4291,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A26:E26">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed cad legislation scraper
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DFA2C1-0005-4B2F-AED3-71B866FF7FC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CA3CA-8459-4530-A738-721C4EABE768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
@@ -3679,7 +3679,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finished cad fed legislator scraper
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844CA3CA-8459-4530-A738-721C4EABE768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4409413E-985B-4F08-B733-4D8B6438DDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
@@ -3679,7 +3679,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added canada fed senate scrape; continued work on cad fed legislation scraper
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4409413E-985B-4F08-B733-4D8B6438DDEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A060DF94-8285-443D-98B5-D8DD70F5FD5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="690" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
@@ -3091,7 +3091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -3679,7 +3679,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added dataclass decorators to legislation row
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36423A93-4C07-4DF8-8AC5-EC733E703155}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838A21EB-2BDF-4D74-AFC4-54C9F08F9E9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23130" yWindow="6945" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -1913,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEEF0DA-C32C-4BCA-97E5-1604306C6773}">
   <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -3091,7 +3091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -3678,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Moved templates to root
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838A21EB-2BDF-4D74-AFC4-54C9F08F9E9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74365D1-9527-4734-A758-A8DCA662F231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>areas_served</t>
   </si>
   <si>
-    <t>phone_number</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -1048,6 +1045,9 @@
   </si>
   <si>
     <t>Priarie, Atlantic</t>
+  </si>
+  <si>
+    <t>phone_numbers</t>
   </si>
 </sst>
 </file>
@@ -1913,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEEF0DA-C32C-4BCA-97E5-1604306C6773}">
   <dimension ref="A1:O114"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1960,7 +1960,7 @@
         <v>61</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I1" s="20" t="s">
         <v>5</v>
@@ -1975,7 +1975,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="20" t="s">
         <v>21</v>
@@ -2007,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I2" s="16" t="s">
         <v>9</v>
@@ -2025,7 +2025,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O2" s="16"/>
     </row>
@@ -2070,7 +2070,7 @@
         <v>34</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O3" s="16"/>
     </row>
@@ -2115,7 +2115,7 @@
         <v>34</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>35</v>
@@ -2162,7 +2162,7 @@
         <v>34</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O5" s="16" t="s">
         <v>33</v>
@@ -2212,7 +2212,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>9</v>
@@ -2230,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O7" s="16" t="s">
         <v>41</v>
@@ -2302,7 +2302,7 @@
         <v>20</v>
       </c>
       <c r="N9" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O9" s="16" t="s">
         <v>51</v>
@@ -2347,7 +2347,7 @@
         <v>34</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O10" s="16" t="s">
         <v>55</v>
@@ -2355,13 +2355,13 @@
     </row>
     <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
@@ -2392,21 +2392,21 @@
         <v>34</v>
       </c>
       <c r="N11" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="D12" s="16"/>
       <c r="E12" s="16" t="s">
@@ -2419,7 +2419,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>9</v>
@@ -2437,24 +2437,24 @@
         <v>20</v>
       </c>
       <c r="N12" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O12" s="16" t="s">
         <v>121</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>9</v>
@@ -2484,15 +2484,15 @@
         <v>34</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>37</v>
@@ -2513,16 +2513,16 @@
     </row>
     <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>130</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -2538,13 +2538,13 @@
     </row>
     <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
@@ -2575,21 +2575,21 @@
         <v>9</v>
       </c>
       <c r="N16" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>137</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>138</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16" t="s">
@@ -2620,21 +2620,21 @@
         <v>34</v>
       </c>
       <c r="N17" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16" t="s">
@@ -2647,7 +2647,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>9</v>
@@ -2665,21 +2665,21 @@
         <v>34</v>
       </c>
       <c r="N18" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>145</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>146</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
@@ -2692,39 +2692,39 @@
         <v>10</v>
       </c>
       <c r="H19" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="M19" s="16" t="s">
+      <c r="N19" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O19" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16" t="s">
@@ -2737,7 +2737,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>9</v>
@@ -2755,21 +2755,21 @@
         <v>20</v>
       </c>
       <c r="N20" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>157</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>158</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16" t="s">
@@ -2797,13 +2797,13 @@
         <v>9</v>
       </c>
       <c r="M21" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="O21" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3091,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,65 +3106,65 @@
   <sheetData>
     <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>69</v>
-      </c>
       <c r="E1" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>257</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>104</v>
-      </c>
       <c r="D4" s="29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E4" s="29">
         <v>43915</v>
@@ -3172,46 +3172,46 @@
     </row>
     <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>193</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>195</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>104</v>
-      </c>
       <c r="D7" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="29">
         <v>43853</v>
@@ -3219,32 +3219,32 @@
     </row>
     <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>198</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3252,73 +3252,73 @@
         <v>21</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="E10" s="29" t="s">
         <v>205</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>208</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>212</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E14" s="29">
         <v>53</v>
@@ -3326,198 +3326,198 @@
     </row>
     <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="29" t="s">
         <v>228</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D16" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>214</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>216</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C19" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>216</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>219</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="29" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="E23" s="29" t="s">
         <v>224</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="24" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="24" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="29" t="s">
         <v>232</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>234</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E27" s="30">
         <v>1</v>
@@ -3525,23 +3525,23 @@
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>273</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B30"/>
       <c r="C30"/>
@@ -3550,31 +3550,31 @@
     </row>
     <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="C31" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="D31" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="31" t="s">
-        <v>69</v>
-      </c>
       <c r="E31" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E32" s="35">
         <v>1</v>
@@ -3582,51 +3582,51 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="E33" s="33" t="s">
         <v>277</v>
-      </c>
-      <c r="E33" s="33" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="C36" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="D36" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="31" t="s">
-        <v>69</v>
-      </c>
       <c r="E36" s="31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" s="32"/>
       <c r="D37" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E37" s="35">
         <v>1</v>
@@ -3634,17 +3634,17 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="E38" s="33" t="s">
         <v>283</v>
-      </c>
-      <c r="E38" s="33" t="s">
-        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -3678,8 +3678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,33 +3694,33 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
@@ -3728,29 +3728,29 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E4" s="4">
         <v>101</v>
@@ -3758,16 +3758,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="E5" s="14">
         <v>43831</v>
@@ -3775,17 +3775,17 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3793,14 +3793,14 @@
         <v>56</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,14 +3808,14 @@
         <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3823,14 +3823,14 @@
         <v>58</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3838,14 +3838,14 @@
         <v>60</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3853,28 +3853,28 @@
         <v>59</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -3882,31 +3882,31 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
@@ -3917,46 +3917,46 @@
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,50 +3964,50 @@
         <v>21</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>63</v>
+        <v>308</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,30 +4015,30 @@
         <v>8</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="E22" s="10">
         <v>24551</v>
@@ -4046,16 +4046,16 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" s="7">
         <v>2</v>
@@ -4063,87 +4063,87 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="E25" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>264</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="C29" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="D29" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="E29" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E30" s="38">
         <v>1</v>
@@ -4151,17 +4151,17 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="40"/>
       <c r="D31" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E31" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4169,16 +4169,16 @@
         <v>62</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="38" t="s">
         <v>92</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -4186,13 +4186,13 @@
         <v>61</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="43" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" s="43" t="s">
         <v>239</v>
-      </c>
-      <c r="D33" s="43" t="s">
-        <v>240</v>
       </c>
       <c r="E33" s="43">
         <v>42</v>
@@ -4200,38 +4200,38 @@
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="C36" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="D36" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="36" t="s">
-        <v>69</v>
-      </c>
       <c r="E36" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E37" s="38">
         <v>1</v>
@@ -4239,47 +4239,47 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="40"/>
       <c r="D38" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="38"/>
       <c r="D39" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="E39" s="38" t="s">
         <v>307</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C40" s="40"/>
       <c r="D40" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="E40" s="40" t="s">
         <v>298</v>
-      </c>
-      <c r="E40" s="40" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -4322,155 +4322,155 @@
   <sheetData>
     <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Q30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Can get most data. Next step is to refactor code, gather committee info and find way to get MORE info from wiki.
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B65F971-7FF6-4D14-BF47-FD34A360940D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7943A6-6B87-42DD-9FA2-71FCDB7D19BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="-27960" yWindow="3885" windowWidth="28080" windowHeight="16440" activeTab="1" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added ca_fed_legislation vote boilerplate
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7943A6-6B87-42DD-9FA2-71FCDB7D19BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C22693-C4CD-4C15-AF3E-D0E738ED143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27960" yWindow="3885" windowWidth="28080" windowHeight="16440" activeTab="1" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -3227,7 +3227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4037,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixes CA fed legislation scraper; pm_party, pm_party_id being inaccurate
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C22693-C4CD-4C15-AF3E-D0E738ED143F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FBFE37-17F9-48AB-8CE2-8B50FAE36B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="-26250" yWindow="3210" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -3227,8 +3227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4037,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added gender data column.
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\github_goverlytics_scrapers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FBFE37-17F9-48AB-8CE2-8B50FAE36B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C899774-6A2F-4EF4-ABE3-2D7CFF323AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26250" yWindow="3210" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="353">
   <si>
     <t>http://www.legislature.state.al.us/aliswww/ISD/ALRepresentative.aspx?NAME=Dismukes&amp;OID_SPONSOR=100570&amp;OID_PERSON=8511</t>
   </si>
@@ -1102,6 +1102,15 @@
   </si>
   <si>
     <t>Bill ID provided by the source website.  Must be unique across the entire site where the data was collected from.</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>M', 'F', 'O'</t>
+  </si>
+  <si>
+    <t>Gender of the legislator. Specified by M (Male), F (Female), or O (Other)</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -1405,12 +1414,106 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1587,13 +1690,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1626,90 +1722,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1724,27 +1736,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E26" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E27" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:E27" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2053,27 +2065,27 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="24" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="15" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.44140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="16" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="15" width="30.109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -2120,7 +2132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -2165,7 +2177,7 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -2210,7 +2222,7 @@
       </c>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
@@ -2257,7 +2269,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -2325,7 +2337,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>38</v>
       </c>
@@ -2372,7 +2384,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>42</v>
       </c>
@@ -2397,7 +2409,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>46</v>
       </c>
@@ -2444,7 +2456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
@@ -2489,7 +2501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>112</v>
       </c>
@@ -2534,7 +2546,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>116</v>
       </c>
@@ -2579,7 +2591,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>121</v>
       </c>
@@ -2626,7 +2638,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>125</v>
       </c>
@@ -2647,7 +2659,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>126</v>
       </c>
@@ -2672,7 +2684,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>133</v>
       </c>
@@ -2717,7 +2729,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>134</v>
       </c>
@@ -2762,7 +2774,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
@@ -2807,7 +2819,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>142</v>
       </c>
@@ -2852,7 +2864,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>149</v>
       </c>
@@ -2897,7 +2909,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>154</v>
       </c>
@@ -2942,20 +2954,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2963,7 +2975,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2971,7 +2983,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2979,7 +2991,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2987,7 +2999,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2995,7 +3007,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3003,7 +3015,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="88" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3011,7 +3023,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="28.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3019,7 +3031,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3027,7 +3039,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3035,7 +3047,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3043,7 +3055,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3051,7 +3063,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3059,7 +3071,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3067,7 +3079,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3075,7 +3087,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -3083,7 +3095,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -3092,7 +3104,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -3100,7 +3112,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -3108,7 +3120,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -3116,7 +3128,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3124,7 +3136,7 @@
       <c r="E102" s="7"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="84.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3132,7 +3144,7 @@
       <c r="E103" s="7"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="87.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3140,7 +3152,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3148,7 +3160,7 @@
       <c r="E105" s="7"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3156,7 +3168,7 @@
       <c r="E106" s="7"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3164,7 +3176,7 @@
       <c r="E107" s="7"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3172,42 +3184,42 @@
       <c r="E108" s="7"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="7"/>
       <c r="C110" s="17"/>
       <c r="D110" s="7"/>
       <c r="E110" s="17"/>
     </row>
-    <row r="111" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="10"/>
     </row>
-    <row r="112" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3231,16 +3243,16 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="62.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
@@ -3257,7 +3269,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>236</v>
       </c>
@@ -3274,7 +3286,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>255</v>
       </c>
@@ -3289,7 +3301,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>170</v>
       </c>
@@ -3306,7 +3318,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>172</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>173</v>
       </c>
@@ -3336,7 +3348,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>186</v>
       </c>
@@ -3353,7 +3365,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>256</v>
       </c>
@@ -3368,7 +3380,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>174</v>
       </c>
@@ -3383,7 +3395,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
@@ -3400,7 +3412,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>175</v>
       </c>
@@ -3415,7 +3427,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>176</v>
       </c>
@@ -3430,7 +3442,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>177</v>
       </c>
@@ -3445,7 +3457,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>221</v>
       </c>
@@ -3460,7 +3472,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>220</v>
       </c>
@@ -3475,7 +3487,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>178</v>
       </c>
@@ -3492,7 +3504,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>179</v>
       </c>
@@ -3509,7 +3521,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>180</v>
       </c>
@@ -3526,7 +3538,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>181</v>
       </c>
@@ -3543,7 +3555,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>182</v>
       </c>
@@ -3556,7 +3568,7 @@
       </c>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>203</v>
       </c>
@@ -3569,7 +3581,7 @@
       </c>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>183</v>
       </c>
@@ -3582,7 +3594,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>184</v>
       </c>
@@ -3599,7 +3611,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>185</v>
       </c>
@@ -3616,7 +3628,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>276</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>187</v>
       </c>
@@ -3646,7 +3658,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>159</v>
       </c>
@@ -3661,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
         <v>163</v>
       </c>
@@ -3676,8 +3688,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
@@ -3686,7 +3698,7 @@
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
@@ -3703,7 +3715,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
         <v>160</v>
       </c>
@@ -3718,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>162</v>
       </c>
@@ -3733,12 +3745,12 @@
         <v>317</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>65</v>
       </c>
@@ -3755,7 +3767,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="44" t="s">
         <v>260</v>
       </c>
@@ -3770,7 +3782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
         <v>261</v>
       </c>
@@ -3785,7 +3797,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="44" t="s">
         <v>278</v>
       </c>
@@ -3800,12 +3812,12 @@
         <v>316</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>65</v>
       </c>
@@ -3822,7 +3834,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
         <v>321</v>
       </c>
@@ -3837,7 +3849,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>322</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
         <v>323</v>
       </c>
@@ -3869,7 +3881,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>324</v>
       </c>
@@ -3884,7 +3896,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
         <v>325</v>
       </c>
@@ -3899,7 +3911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>326</v>
       </c>
@@ -3914,7 +3926,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
         <v>327</v>
       </c>
@@ -3929,7 +3941,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="33" t="s">
         <v>340</v>
       </c>
@@ -3944,7 +3956,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
         <v>328</v>
       </c>
@@ -3963,62 +3975,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E28">
-    <cfRule type="expression" dxfId="26" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:E33">
-    <cfRule type="expression" dxfId="25" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:E38">
-    <cfRule type="expression" dxfId="24" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:E39">
-    <cfRule type="expression" dxfId="23" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:E44">
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:E45">
-    <cfRule type="expression" dxfId="21" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:E46">
-    <cfRule type="expression" dxfId="20" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:E48 A47:C47 E47">
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E49">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:E50">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:E51">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4035,23 +4047,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="37.5546875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="68.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
@@ -4068,7 +4080,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>236</v>
       </c>
@@ -4085,7 +4097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>255</v>
       </c>
@@ -4100,7 +4112,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>237</v>
       </c>
@@ -4115,7 +4127,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
@@ -4132,7 +4144,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>256</v>
       </c>
@@ -4147,7 +4159,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -4162,7 +4174,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -4177,7 +4189,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -4192,7 +4204,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
@@ -4207,7 +4219,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>159</v>
       </c>
@@ -4239,7 +4251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
@@ -4254,7 +4266,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>161</v>
       </c>
@@ -4271,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -4286,7 +4298,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -4301,418 +4313,433 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>169</v>
+        <v>280</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E22" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>24551</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E24" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7" t="s">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="34" t="s">
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A29" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B30" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C30" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D30" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E30" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B30" s="38" t="s">
+      <c r="B31" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C31" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D31" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E31" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="39" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B32" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40" t="s">
+      <c r="C32" s="40"/>
+      <c r="D32" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E32" s="40" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B33" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C33" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="38" t="s">
+      <c r="D33" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E33" s="38" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
+    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B34" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C34" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D33" s="43" t="s">
+      <c r="D34" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E34" s="43">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="34" t="s">
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A36" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B37" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C37" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D37" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E37" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B38" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C38" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D38" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E38" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B39" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="43" t="s">
+      <c r="C39" s="40"/>
+      <c r="D39" s="43" t="s">
         <v>299</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E39" s="40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B40" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38" t="s">
+      <c r="C40" s="38"/>
+      <c r="D40" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="E39" s="38" t="s">
+      <c r="E40" s="38" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B41" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="40" t="s">
+      <c r="C41" s="40"/>
+      <c r="D41" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E41" s="40" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="39"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A43" s="34" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="39"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+    </row>
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A44" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B45" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C45" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="D45" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E45" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B46" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="38" t="s">
+      <c r="C46" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="D45" s="38" t="s">
+      <c r="D46" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E46" s="38" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="39" t="s">
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B47" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="40" t="s">
+      <c r="C47" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="D46" s="43" t="s">
+      <c r="D47" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="E46" s="43" t="s">
+      <c r="E47" s="43" t="s">
         <v>288</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A26:E26">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="A27:E27">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E21" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
-    <hyperlink ref="C21" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
+    <hyperlink ref="C22" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4730,182 +4757,182 @@
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="27" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A16" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A23" s="26" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A38" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>346</v>
       </c>

</xml_diff>

<commit_message>
Insertion for wiki_url for legislators.
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C899774-6A2F-4EF4-ABE3-2D7CFF323AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F574FA69-A1AB-4560-B897-8A83B044BD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="357">
   <si>
     <t>http://www.legislature.state.al.us/aliswww/ISD/ALRepresentative.aspx?NAME=Dismukes&amp;OID_SPONSOR=100570&amp;OID_PERSON=8511</t>
   </si>
@@ -1111,6 +1111,18 @@
   </si>
   <si>
     <t>Gender of the legislator. Specified by M (Male), F (Female), or O (Other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT </t>
+  </si>
+  <si>
+    <t>wiki_url (UNIQUE)</t>
+  </si>
+  <si>
+    <t>Wikipedia URL for the legislator, used to uniquely identify legislators across the country</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Jeremy_Harper_(politician)</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1761,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E27" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:E27" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E28" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:E28" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="16"/>
@@ -2065,27 +2077,27 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="24" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="15" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" style="2" customWidth="1"/>
     <col min="14" max="14" width="16" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="2"/>
+    <col min="15" max="15" width="30.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -2132,7 +2144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -2177,7 +2189,7 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -2222,7 +2234,7 @@
       </c>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
@@ -2269,7 +2281,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
@@ -2316,7 +2328,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -2337,7 +2349,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>38</v>
       </c>
@@ -2384,7 +2396,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>42</v>
       </c>
@@ -2409,7 +2421,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>46</v>
       </c>
@@ -2456,7 +2468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
@@ -2501,7 +2513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>112</v>
       </c>
@@ -2546,7 +2558,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>116</v>
       </c>
@@ -2591,7 +2603,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>121</v>
       </c>
@@ -2638,7 +2650,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>125</v>
       </c>
@@ -2659,7 +2671,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>126</v>
       </c>
@@ -2684,7 +2696,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>133</v>
       </c>
@@ -2729,7 +2741,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>134</v>
       </c>
@@ -2774,7 +2786,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
@@ -2819,7 +2831,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>142</v>
       </c>
@@ -2864,7 +2876,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>149</v>
       </c>
@@ -2909,7 +2921,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>154</v>
       </c>
@@ -2954,20 +2966,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2975,7 +2987,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2983,7 +2995,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2991,7 +3003,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2999,7 +3011,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3007,7 +3019,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3015,7 +3027,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="88" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3023,7 +3035,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" ht="28.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3031,7 +3043,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3039,7 +3051,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3047,7 +3059,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3055,7 +3067,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3063,7 +3075,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3071,7 +3083,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3079,7 +3091,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3087,7 +3099,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -3095,7 +3107,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -3104,7 +3116,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -3112,7 +3124,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -3120,7 +3132,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -3128,7 +3140,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3136,7 +3148,7 @@
       <c r="E102" s="7"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="84.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3144,7 +3156,7 @@
       <c r="E103" s="7"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="87.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3152,7 +3164,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3160,7 +3172,7 @@
       <c r="E105" s="7"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3168,7 +3180,7 @@
       <c r="E106" s="7"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3176,7 +3188,7 @@
       <c r="E107" s="7"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3184,42 +3196,42 @@
       <c r="E108" s="7"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="7"/>
       <c r="C110" s="17"/>
       <c r="D110" s="7"/>
       <c r="E110" s="17"/>
     </row>
-    <row r="111" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="10"/>
     </row>
-    <row r="112" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3243,16 +3255,16 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="58.33203125" customWidth="1"/>
-    <col min="5" max="5" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
@@ -3269,7 +3281,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>236</v>
       </c>
@@ -3286,7 +3298,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>255</v>
       </c>
@@ -3301,7 +3313,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>170</v>
       </c>
@@ -3318,7 +3330,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>172</v>
       </c>
@@ -3333,7 +3345,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>173</v>
       </c>
@@ -3348,7 +3360,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>186</v>
       </c>
@@ -3365,7 +3377,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>256</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>174</v>
       </c>
@@ -3395,7 +3407,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
@@ -3412,7 +3424,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>175</v>
       </c>
@@ -3427,7 +3439,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>176</v>
       </c>
@@ -3442,7 +3454,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>177</v>
       </c>
@@ -3457,7 +3469,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>221</v>
       </c>
@@ -3472,7 +3484,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>220</v>
       </c>
@@ -3487,7 +3499,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>178</v>
       </c>
@@ -3504,7 +3516,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>179</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>180</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>181</v>
       </c>
@@ -3555,7 +3567,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>182</v>
       </c>
@@ -3568,7 +3580,7 @@
       </c>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>203</v>
       </c>
@@ -3581,7 +3593,7 @@
       </c>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>183</v>
       </c>
@@ -3594,7 +3606,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>184</v>
       </c>
@@ -3611,7 +3623,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>185</v>
       </c>
@@ -3628,7 +3640,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>276</v>
       </c>
@@ -3643,7 +3655,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>187</v>
       </c>
@@ -3658,7 +3670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>159</v>
       </c>
@@ -3673,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>163</v>
       </c>
@@ -3688,8 +3700,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
@@ -3698,7 +3710,7 @@
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
@@ -3715,7 +3727,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>160</v>
       </c>
@@ -3730,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>162</v>
       </c>
@@ -3745,12 +3757,12 @@
         <v>317</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>65</v>
       </c>
@@ -3767,7 +3779,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>260</v>
       </c>
@@ -3782,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>261</v>
       </c>
@@ -3797,7 +3809,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>278</v>
       </c>
@@ -3812,12 +3824,12 @@
         <v>316</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>65</v>
       </c>
@@ -3834,7 +3846,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>321</v>
       </c>
@@ -3849,7 +3861,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
         <v>322</v>
       </c>
@@ -3866,7 +3878,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
         <v>323</v>
       </c>
@@ -3881,7 +3893,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>324</v>
       </c>
@@ -3896,7 +3908,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
         <v>325</v>
       </c>
@@ -3911,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>326</v>
       </c>
@@ -3926,7 +3938,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
         <v>327</v>
       </c>
@@ -3941,7 +3953,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
         <v>340</v>
       </c>
@@ -3956,7 +3968,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
         <v>328</v>
       </c>
@@ -4047,23 +4059,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="68.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="24"/>
+    <col min="1" max="1" width="37.5703125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="60.28515625" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
@@ -4080,7 +4092,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>236</v>
       </c>
@@ -4097,7 +4109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>255</v>
       </c>
@@ -4112,7 +4124,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>237</v>
       </c>
@@ -4127,7 +4139,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
@@ -4144,7 +4156,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>256</v>
       </c>
@@ -4159,7 +4171,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -4174,7 +4186,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -4189,7 +4201,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -4204,7 +4216,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
@@ -4219,7 +4231,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -4234,7 +4246,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>159</v>
       </c>
@@ -4251,7 +4263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
@@ -4266,7 +4278,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>161</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -4298,7 +4310,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -4313,7 +4325,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>350</v>
       </c>
@@ -4328,418 +4340,433 @@
         <v>351</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>92</v>
+        <v>232</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>169</v>
+        <v>280</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E23" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E24" s="10">
         <v>24551</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E25" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A29" s="34" t="s">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B31" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C31" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D31" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E31" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="37" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B32" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C32" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D32" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E32" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="39" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B33" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40" t="s">
+      <c r="C33" s="40"/>
+      <c r="D33" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E33" s="40" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B34" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C34" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D34" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E34" s="38" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="42" t="s">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B35" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C35" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D35" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E35" s="43">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A36" s="34" t="s">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
+    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B38" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C38" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D38" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E38" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B39" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C39" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D39" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E39" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="39" t="s">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B40" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="43" t="s">
+      <c r="C40" s="40"/>
+      <c r="D40" s="43" t="s">
         <v>299</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E40" s="40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B41" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38" t="s">
+      <c r="C41" s="38"/>
+      <c r="D41" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E41" s="38" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B42" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40" t="s">
+      <c r="C42" s="40"/>
+      <c r="D42" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E42" s="40" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-    </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A44" s="34" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="36" t="s">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B46" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C46" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D46" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E46" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B47" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C47" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D47" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="E46" s="38" t="s">
+      <c r="E47" s="38" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="39" t="s">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B48" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C48" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D48" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E48" s="43" t="s">
         <v>288</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A27:E27">
+  <conditionalFormatting sqref="A28:E28">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E22" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
-    <hyperlink ref="C22" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
+    <hyperlink ref="E23" r:id="rId1" xr:uid="{7F13F44F-EB42-4630-8911-221C4CEB1D41}"/>
+    <hyperlink ref="C23" r:id="rId2" xr:uid="{D69EBFBA-8B42-405B-B535-1043B77152D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4757,182 +4784,182 @@
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="27" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A38" s="26" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>346</v>
       </c>

</xml_diff>

<commit_message>
Added definition for is_active for legislators
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d35ac2d39d6bf01d/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{AC524DE6-7BF7-4B35-B035-CF8AFB79B9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D42214E0-3608-4414-A047-E44FBAB56412}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8454EE4-4044-4598-867D-DE566731A180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="1740" windowWidth="13725" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" firstSheet="1" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
     <sheet name="legislation_data_dictionary" sheetId="4" r:id="rId2"/>
-    <sheet name="Video Analysis Tool" sheetId="6" r:id="rId3"/>
-    <sheet name="change log" sheetId="5" r:id="rId4"/>
-    <sheet name="legislators_data_dictionary" sheetId="3" r:id="rId5"/>
+    <sheet name="change log" sheetId="5" r:id="rId3"/>
+    <sheet name="legislators_data_dictionary" sheetId="3" r:id="rId4"/>
+    <sheet name="Video Analysis Tool" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="375">
   <si>
     <t>http://www.legislature.state.al.us/aliswww/ISD/ALRepresentative.aspx?NAME=Dismukes&amp;OID_SPONSOR=100570&amp;OID_PERSON=8511</t>
   </si>
@@ -1182,6 +1181,15 @@
   </si>
   <si>
     <t>{information, foreign relations, public lands,}</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Indicates whether the legislator is currently holding a seat.</t>
   </si>
 </sst>
 </file>
@@ -1496,14 +1504,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -1824,27 +1825,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E27" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:E27" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:E28" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4063,62 +4064,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E28">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:E33">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:E38">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:E39">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:E44">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:E45">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:E46">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:E48 A47:C47 E47">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E49">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:E50">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:E51">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4134,217 +4135,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503CA815-CFA2-4022-854C-51060F5A3A5E}">
-  <dimension ref="A1:E18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>355</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>355</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>359</v>
-      </c>
-      <c r="E3" s="48">
-        <v>47861</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>364</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>365</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>357</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>366</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>367</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:E18">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C073D259-A667-418B-8FFC-7962EC73964E}">
   <dimension ref="A1:A43"/>
   <sheetViews>
@@ -4537,12 +4327,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4988,244 +4778,259 @@
         <v>251</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="E28" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B31" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C31" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D31" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E31" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B32" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C32" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D32" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E32" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B33" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40" t="s">
+      <c r="C33" s="40"/>
+      <c r="D33" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E33" s="40" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B34" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C34" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D34" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E34" s="38" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B35" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C35" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D35" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E35" s="43">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="34" t="s">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B38" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C38" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D38" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E38" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B39" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C39" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D39" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E39" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
         <v>261</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B40" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="43" t="s">
+      <c r="C40" s="40"/>
+      <c r="D40" s="43" t="s">
         <v>299</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E40" s="40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B41" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38" t="s">
+      <c r="C41" s="38"/>
+      <c r="D41" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E41" s="38" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B42" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40" t="s">
+      <c r="C42" s="40"/>
+      <c r="D42" s="40" t="s">
         <v>272</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E42" s="40" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-    </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A44" s="34" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="39"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A45" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B46" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C46" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="36" t="s">
+      <c r="D46" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E46" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B47" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C47" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D47" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="E46" s="38" t="s">
+      <c r="E47" s="38" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="39" t="s">
         <v>285</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B48" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C48" s="40" t="s">
         <v>286</v>
       </c>
-      <c r="D47" s="43" t="s">
+      <c r="D48" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="E47" s="43" t="s">
+      <c r="E48" s="43" t="s">
         <v>288</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A27:E27">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A27:E28">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5239,4 +5044,215 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503CA815-CFA2-4022-854C-51060F5A3A5E}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" s="48">
+        <v>47861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>367</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:E18">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"Changed definition for region."
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8454EE4-4044-4598-867D-DE566731A180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EE7F66-BF18-4FF5-A211-88B4C5942D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" firstSheet="1" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
@@ -946,9 +946,6 @@
     <t>Generated by the initialize_row function. Name of legislator province/territory</t>
   </si>
   <si>
-    <t>Can be acquired by calling get_region(prov_terr_abbreviation). Region of the legislator's home province.</t>
-  </si>
-  <si>
     <t>Generated by database in insert query. Used to uniquely identify each legislator.</t>
   </si>
   <si>
@@ -1190,6 +1187,9 @@
   </si>
   <si>
     <t>Indicates whether the legislator is currently holding a seat.</t>
+  </si>
+  <si>
+    <t>Generated by the initialize_row function. Region of the legislator's home province.</t>
   </si>
 </sst>
 </file>
@@ -1513,97 +1513,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1779,6 +1688,13 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1811,6 +1727,90 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1825,27 +1825,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DA97D88-36C1-40F2-8446-3F74C2F25EFA}" name="Table2" displayName="Table2" ref="A1:E28" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{6EDE9B04-AD64-4005-946C-65512677CD01}" name="Field" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{64DB1534-BA61-40E3-B47F-11C894DBC398}" name="Data Type" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{2659A690-3026-482E-8788-AA1C64B52F86}" name="Data Format" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{2723E5CF-ED75-4F94-B6C1-47D7FE424FA1}" name="Description" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{7BD3D5B3-00DC-4AB2-979E-FEB88D6F531C}" name="Examples" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53E3B775-AF75-4D9C-BC87-1A27898A6C8F}" name="Table3" displayName="Table3" ref="A1:E28" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:E28" xr:uid="{A3DB6754-321C-4EF3-998D-49CBAAF7FD5E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{B67739BF-A33D-4601-8DB0-546444D3D0D0}" name="Field" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7E697C33-D281-42B6-A40B-93EC8EE2EB09}" name="Data Type" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{71843A29-530B-49B4-A58D-BA2B595C7289}" name="Data Format" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{6A0A1AFD-AAC2-4892-A637-BCCB9DC153C7}" name="Description" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{1FEC4AA1-A8BB-4159-86D3-C17CF3ECE709}" name="Examples" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2154,27 +2154,27 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.44140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="24" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="15" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.44140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="16" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="15" width="30.109375" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>38</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>42</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>46</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>112</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>116</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>121</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>125</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>126</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>133</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>134</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>149</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>154</v>
       </c>
@@ -3043,20 +3043,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3064,7 +3064,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3072,7 +3072,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3080,7 +3080,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3088,7 +3088,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3096,7 +3096,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3104,7 +3104,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="88" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3112,7 +3112,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="28.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3120,7 +3120,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3128,7 +3128,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3136,7 +3136,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3144,7 +3144,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3152,7 +3152,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3160,7 +3160,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3168,7 +3168,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3176,7 +3176,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -3184,7 +3184,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -3193,7 +3193,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -3201,7 +3201,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -3209,7 +3209,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -3217,7 +3217,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3225,7 +3225,7 @@
       <c r="E102" s="7"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="84.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3233,7 +3233,7 @@
       <c r="E103" s="7"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="87.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3241,7 +3241,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3249,7 +3249,7 @@
       <c r="E105" s="7"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3257,7 +3257,7 @@
       <c r="E106" s="7"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3265,7 +3265,7 @@
       <c r="E107" s="7"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3273,42 +3273,42 @@
       <c r="E108" s="7"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="7"/>
       <c r="C110" s="17"/>
       <c r="D110" s="7"/>
       <c r="E110" s="17"/>
     </row>
-    <row r="111" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="10"/>
     </row>
-    <row r="112" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3332,16 +3332,16 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.33203125" customWidth="1"/>
+    <col min="5" max="5" width="62.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>236</v>
       </c>
@@ -3369,13 +3369,13 @@
         <v>189</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>255</v>
       </c>
@@ -3384,13 +3384,13 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>170</v>
       </c>
@@ -3401,13 +3401,13 @@
         <v>102</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="29">
         <v>43915</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>172</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>173</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>186</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>256</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>174</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>175</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>176</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>177</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>221</v>
       </c>
@@ -3555,13 +3555,13 @@
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E14" s="29">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>220</v>
       </c>
@@ -3570,13 +3570,13 @@
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>178</v>
       </c>
@@ -3587,13 +3587,13 @@
         <v>90</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
         <v>179</v>
       </c>
@@ -3604,13 +3604,13 @@
         <v>211</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>180</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>181</v>
       </c>
@@ -3638,13 +3638,13 @@
         <v>211</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
         <v>182</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
         <v>203</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">
         <v>183</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>184</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>185</v>
       </c>
@@ -3714,10 +3714,10 @@
         <v>223</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>276</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
         <v>187</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="29" t="s">
         <v>159</v>
       </c>
@@ -3756,13 +3756,13 @@
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E27" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
         <v>163</v>
       </c>
@@ -3771,14 +3771,14 @@
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
@@ -3787,7 +3787,7 @@
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
         <v>160</v>
       </c>
@@ -3813,13 +3813,13 @@
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E32" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>162</v>
       </c>
@@ -3828,18 +3828,18 @@
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>65</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="44" t="s">
         <v>260</v>
       </c>
@@ -3865,13 +3865,13 @@
       </c>
       <c r="C37" s="44"/>
       <c r="D37" s="44" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E37" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
         <v>261</v>
       </c>
@@ -3880,13 +3880,13 @@
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="44" t="s">
         <v>278</v>
       </c>
@@ -3895,18 +3895,18 @@
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="E39" s="45" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>65</v>
       </c>
@@ -3923,24 +3923,24 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B43" s="44" t="s">
         <v>71</v>
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="E43" s="45" t="s">
         <v>329</v>
       </c>
-      <c r="E43" s="45" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B44" s="33" t="s">
         <v>71</v>
@@ -3949,177 +3949,177 @@
         <v>230</v>
       </c>
       <c r="D44" s="33" t="s">
+        <v>330</v>
+      </c>
+      <c r="E44" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="E44" s="33" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B45" s="44" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="E45" s="45" t="s">
         <v>333</v>
       </c>
-      <c r="E45" s="45" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B46" s="33" t="s">
         <v>71</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="E46" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="E46" s="33" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B47" s="44" t="s">
         <v>257</v>
       </c>
       <c r="C47" s="44"/>
       <c r="D47" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E47" s="45">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B48" s="33" t="s">
         <v>257</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E48" s="33">
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B49" s="44" t="s">
         <v>257</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="E49" s="45" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="33" t="s">
         <v>339</v>
-      </c>
-      <c r="E49" s="45" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="33" t="s">
-        <v>340</v>
       </c>
       <c r="B50" s="33" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="E50" s="33" t="s">
         <v>341</v>
       </c>
-      <c r="E50" s="33" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B51" s="44" t="s">
         <v>89</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D51" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="E51" s="45" t="s">
         <v>343</v>
-      </c>
-      <c r="E51" s="45" t="s">
-        <v>344</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E28">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="27" priority="12">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:E33">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="26" priority="11">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:E38">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:E39">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="24" priority="9">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:E44">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:E45">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="22" priority="7">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:E46">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="21" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:E48 A47:C47 E47">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E49">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:E50">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:E51">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4142,184 +4142,184 @@
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="27" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A16" s="26" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A23" s="26" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A38" s="26" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="25" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -4331,21 +4331,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="24" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="37.5546875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="41.5546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="68.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>236</v>
       </c>
@@ -4373,13 +4373,13 @@
         <v>70</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>255</v>
       </c>
@@ -4388,13 +4388,13 @@
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>237</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
@@ -4420,13 +4420,13 @@
         <v>102</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E5" s="14">
         <v>43831</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>256</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>159</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>161</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -4580,7 +4580,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -4595,22 +4595,22 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>64</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>280</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>169</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>24551</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>97</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>98</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>249</v>
       </c>
@@ -4778,27 +4778,27 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>373</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E28" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A31" s="36" t="s">
         <v>65</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="37" t="s">
         <v>160</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="39" t="s">
         <v>162</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="37" t="s">
         <v>62</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="42" t="s">
         <v>61</v>
       </c>
@@ -4881,12 +4881,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A38" s="36" t="s">
         <v>65</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="37" t="s">
         <v>260</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="39" t="s">
         <v>261</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="37" t="s">
         <v>278</v>
       </c>
@@ -4944,13 +4944,13 @@
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="38" t="s">
-        <v>300</v>
+        <v>374</v>
       </c>
       <c r="E41" s="38" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>271</v>
       </c>
@@ -4965,19 +4965,19 @@
         <v>273</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="39"/>
       <c r="B43" s="40"/>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
     </row>
-    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A45" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="36" t="s">
         <v>65</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="37" t="s">
         <v>284</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
         <v>285</v>
       </c>
@@ -5030,7 +5030,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A27:E28">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5054,16 +5054,16 @@
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>65</v>
       </c>
@@ -5077,90 +5077,90 @@
         <v>68</v>
       </c>
       <c r="E1" s="31" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="B2" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>355</v>
-      </c>
       <c r="B3" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>102</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E3" s="48">
         <v>47861</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B4" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>364</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>365</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>366</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>367</v>
-      </c>
       <c r="E7" s="33" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>71</v>
       </c>
@@ -5168,79 +5168,79 @@
         <v>89</v>
       </c>
       <c r="C8" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
       <c r="E16" s="32"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>

</xml_diff>

<commit_message>
pushed change log to end of excel.
</commit_message>
<xml_diff>
--- a/dataDictionary.xlsx
+++ b/dataDictionary.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\Work\goverlytics-scrapers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EE7F66-BF18-4FF5-A211-88B4C5942D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A886288-F3B0-4606-B71E-CD870C7218FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="3" xr2:uid="{3A0A1172-2B9D-4961-A408-E801DAC38027}"/>
   </bookViews>
   <sheets>
     <sheet name="legislators" sheetId="1" r:id="rId1"/>
     <sheet name="legislation_data_dictionary" sheetId="4" r:id="rId2"/>
-    <sheet name="change log" sheetId="5" r:id="rId3"/>
-    <sheet name="legislators_data_dictionary" sheetId="3" r:id="rId4"/>
-    <sheet name="Video Analysis Tool" sheetId="6" r:id="rId5"/>
+    <sheet name="legislators_data_dictionary" sheetId="3" r:id="rId3"/>
+    <sheet name="Video Analysis Tool" sheetId="6" r:id="rId4"/>
+    <sheet name="change log" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2154,27 +2154,27 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="24" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="15" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" style="2" customWidth="1"/>
     <col min="14" max="14" width="16" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="2"/>
+    <col min="15" max="15" width="30.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="21" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="O3" s="16"/>
     </row>
-    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>36</v>
       </c>
@@ -2426,7 +2426,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>38</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>42</v>
       </c>
@@ -2498,7 +2498,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>46</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>52</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>112</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>116</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>121</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>125</v>
       </c>
@@ -2748,7 +2748,7 @@
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>126</v>
       </c>
@@ -2773,7 +2773,7 @@
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>133</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>134</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>149</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>154</v>
       </c>
@@ -3043,20 +3043,20 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3064,7 +3064,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3072,7 +3072,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3080,7 +3080,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3088,7 +3088,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3096,7 +3096,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3104,7 +3104,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="88" spans="1:6" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3112,7 +3112,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" ht="28.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="28.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3120,7 +3120,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3128,7 +3128,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3136,7 +3136,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3144,7 +3144,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3152,7 +3152,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3160,7 +3160,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3168,7 +3168,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3176,7 +3176,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -3184,7 +3184,7 @@
       <c r="E97" s="9"/>
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -3193,7 +3193,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="11"/>
     </row>
-    <row r="99" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -3201,7 +3201,7 @@
       <c r="E99" s="9"/>
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -3209,7 +3209,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -3217,7 +3217,7 @@
       <c r="E101" s="9"/>
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3225,7 +3225,7 @@
       <c r="E102" s="7"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="84.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3233,7 +3233,7 @@
       <c r="E103" s="7"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="87.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3241,7 +3241,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3249,7 +3249,7 @@
       <c r="E105" s="7"/>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3257,7 +3257,7 @@
       <c r="E106" s="7"/>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3265,7 +3265,7 @@
       <c r="E107" s="7"/>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3273,42 +3273,42 @@
       <c r="E108" s="7"/>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="1:7" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="B110" s="7"/>
       <c r="C110" s="17"/>
       <c r="D110" s="7"/>
       <c r="E110" s="17"/>
     </row>
-    <row r="111" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="10"/>
     </row>
-    <row r="112" spans="1:7" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
     </row>
-    <row r="113" spans="1:5" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3328,20 +3328,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64B5988-2829-4E33-B80D-452332585A28}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" customWidth="1"/>
-    <col min="4" max="4" width="58.33203125" customWidth="1"/>
-    <col min="5" max="5" width="62.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>65</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>236</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>255</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>170</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>43915</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>172</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="24" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>173</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>186</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>43853</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>256</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>174</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>21</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>175</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>176</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>177</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="24" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>221</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>220</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>178</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="24" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>179</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>180</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>181</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>182</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>203</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>183</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="24" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>184</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" s="24" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>185</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="24" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>276</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="24" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>187</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="24" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
         <v>159</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>163</v>
       </c>
@@ -3777,8 +3777,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:5" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
@@ -3787,7 +3787,7 @@
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>65</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>160</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>162</v>
       </c>
@@ -3834,12 +3834,12 @@
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>65</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>260</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>261</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>278</v>
       </c>
@@ -3901,12 +3901,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>65</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
         <v>320</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
         <v>321</v>
       </c>
@@ -3955,7 +3955,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
         <v>322</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>323</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
         <v>324</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>325</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
         <v>326</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="33" t="s">
         <v>339</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
         <v>327</v>
       </c>
@@ -4135,217 +4135,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C073D259-A667-418B-8FFC-7962EC73964E}">
-  <dimension ref="A1:A43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="27" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A16" s="26" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A23" s="26" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="41" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A38" s="26" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>345</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55107144-B800-4539-84B8-6CE1FD45F7F7}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="41.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="68.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="24"/>
+    <col min="1" max="1" width="37.5703125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="60.28515625" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>65</v>
       </c>
@@ -4362,7 +4169,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>236</v>
       </c>
@@ -4379,7 +4186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>255</v>
       </c>
@@ -4394,7 +4201,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>237</v>
       </c>
@@ -4409,7 +4216,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>170</v>
       </c>
@@ -4426,7 +4233,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>256</v>
       </c>
@@ -4441,7 +4248,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>56</v>
       </c>
@@ -4456,7 +4263,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>57</v>
       </c>
@@ -4471,7 +4278,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -4486,7 +4293,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
@@ -4501,7 +4308,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>59</v>
       </c>
@@ -4516,7 +4323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>159</v>
       </c>
@@ -4533,7 +4340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>163</v>
       </c>
@@ -4548,7 +4355,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>161</v>
       </c>
@@ -4565,7 +4372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -4580,7 +4387,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>63</v>
       </c>
@@ -4595,7 +4402,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>349</v>
       </c>
@@ -4610,7 +4417,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>64</v>
       </c>
@@ -4627,7 +4434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
@@ -4644,7 +4451,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>280</v>
       </c>
@@ -4661,7 +4468,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>169</v>
       </c>
@@ -4678,7 +4485,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>8</v>
       </c>
@@ -4695,7 +4502,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -4712,7 +4519,7 @@
         <v>24551</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>97</v>
       </c>
@@ -4729,7 +4536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>98</v>
       </c>
@@ -4746,7 +4553,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>99</v>
       </c>
@@ -4763,7 +4570,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>249</v>
       </c>
@@ -4778,7 +4585,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>371</v>
       </c>
@@ -4793,12 +4600,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
         <v>65</v>
       </c>
@@ -4815,7 +4622,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>160</v>
       </c>
@@ -4832,7 +4639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
         <v>162</v>
       </c>
@@ -4847,7 +4654,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="37" t="s">
         <v>62</v>
       </c>
@@ -4864,7 +4671,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>61</v>
       </c>
@@ -4881,12 +4688,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="34" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="36" t="s">
         <v>65</v>
       </c>
@@ -4903,7 +4710,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
         <v>260</v>
       </c>
@@ -4920,7 +4727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
         <v>261</v>
       </c>
@@ -4935,7 +4742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
         <v>278</v>
       </c>
@@ -4950,7 +4757,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>271</v>
       </c>
@@ -4965,19 +4772,19 @@
         <v>273</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="39"/>
       <c r="B43" s="40"/>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
     </row>
-    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="34" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
         <v>65</v>
       </c>
@@ -4994,7 +4801,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="37" t="s">
         <v>284</v>
       </c>
@@ -5011,7 +4818,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="39" t="s">
         <v>285</v>
       </c>
@@ -5046,24 +4853,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503CA815-CFA2-4022-854C-51060F5A3A5E}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>65</v>
       </c>
@@ -5080,7 +4887,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>353</v>
       </c>
@@ -5097,7 +4904,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>354</v>
       </c>
@@ -5114,7 +4921,7 @@
         <v>47861</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>355</v>
       </c>
@@ -5127,14 +4934,14 @@
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="32" t="s">
@@ -5143,7 +4950,7 @@
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>356</v>
       </c>
@@ -5160,7 +4967,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>71</v>
       </c>
@@ -5177,70 +4984,70 @@
         <v>368</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
       <c r="E16" s="32"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
@@ -5255,4 +5062,197 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C073D259-A667-418B-8FFC-7962EC73964E}">
+  <dimension ref="A1:A43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A23" s="26" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A38" s="26" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>